<commit_message>
solved day 21 part 2
</commit_message>
<xml_diff>
--- a/days/wip/day21/day21.xlsx
+++ b/days/wip/day21/day21.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmgimeno/Projects-Java/aoc2023/days/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmgimeno/Projects-Java/aoc2023/days/wip/day21/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C594D18E-67CB-534D-8F68-48BE1B133D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29514E64-1CAD-3949-A37A-BBAA2AFE7B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" activeTab="2" xr2:uid="{BF4CD24C-F416-FA4E-B6A7-B2708D50FA3E}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" activeTab="1" xr2:uid="{BF4CD24C-F416-FA4E-B6A7-B2708D50FA3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="day21_input_500" localSheetId="1">Input!$A$1:$B$501</definedName>
     <definedName name="day21_input_500" localSheetId="2">'Input-diffs'!$A$2:$B$502</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +45,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{7E1197DD-536C-1D49-9E15-4C89588914CA}" name="day21-example-500" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/jmgimeno/Projects-Java/aoc2023/days/day21-example-500.csv" decimal="," thousands="." tab="0" semicolon="1">
+    <textPr sourceFile="/Users/jmgimeno/Projects-Java/aoc2023/days/day21-example-500.csv" decimal="," thousands="." tab="0" semicolon="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -53,7 +53,7 @@
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{969071E6-2A63-4E4C-9676-8CC8DD761489}" name="day21-input-500" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/jmgimeno/Projects-Java/aoc2023/days/day21-input-500.csv" decimal="," thousands="." tab="0" semicolon="1">
+    <textPr sourceFile="/Users/jmgimeno/Projects-Java/aoc2023/days/day21-input-500.csv" decimal="," thousands="." tab="0" semicolon="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -61,7 +61,7 @@
     </textPr>
   </connection>
   <connection id="3" xr16:uid="{2B2B0BE3-2B51-314F-A72F-2E28859ADA7E}" name="day21-input-5001" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/jmgimeno/Projects-Java/aoc2023/days/day21-input-500.csv" decimal="," thousands="." tab="0" semicolon="1">
+    <textPr sourceFile="/Users/jmgimeno/Projects-Java/aoc2023/days/day21-input-500.csv" decimal="," thousands="." tab="0" semicolon="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>step</t>
   </si>
@@ -94,6 +94,15 @@
   <si>
     <t>diff5</t>
   </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
 </sst>
 </file>
 
@@ -108,15 +117,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -124,12 +145,82 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12200,16 +12291,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{697BB0DA-9B3F-D842-AFE4-E10728BE28DB}">
-  <dimension ref="A1:B501"/>
+  <dimension ref="A1:I501"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -12340,7 +12432,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -12348,7 +12440,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -12356,7 +12448,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -12364,7 +12456,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -12372,7 +12464,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -12380,7 +12472,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -12388,7 +12480,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -12396,7 +12488,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -12404,7 +12496,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -12412,7 +12504,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -12420,7 +12512,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -12428,39 +12520,100 @@
         <v>633</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
         <v>662</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>65</v>
+      </c>
+      <c r="F28">
+        <v>3742</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I28" s="4">
+        <f>F29-F28-I29</f>
+        <v>14881</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
         <v>733</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>196</v>
+      </c>
+      <c r="F29">
+        <v>33564</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I29" s="6">
+        <f>(4*F29-3*F28-F30)/2</f>
+        <v>14941</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
         <v>763</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>327</v>
+      </c>
+      <c r="F30">
+        <v>93148</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I30" s="8">
+        <f>F28</f>
+        <v>3742</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
         <v>843</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <v>458</v>
+      </c>
+      <c r="F31">
+        <v>182494</v>
+      </c>
+      <c r="I31">
+        <f>I28*9+3*I29+I30</f>
+        <v>182494</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -12733,10 +12886,10 @@
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66">
+      <c r="A66" s="1">
         <v>65</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="1">
         <v>3742</v>
       </c>
     </row>
@@ -13781,10 +13934,10 @@
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A197">
+      <c r="A197" s="1">
         <v>196</v>
       </c>
-      <c r="B197">
+      <c r="B197" s="1">
         <v>33564</v>
       </c>
     </row>
@@ -14829,10 +14982,10 @@
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A328">
+      <c r="A328" s="1">
         <v>327</v>
       </c>
-      <c r="B328">
+      <c r="B328" s="1">
         <v>93148</v>
       </c>
     </row>
@@ -15877,10 +16030,10 @@
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A459">
+      <c r="A459" s="2">
         <v>458</v>
       </c>
-      <c r="B459">
+      <c r="B459" s="2">
         <v>182494</v>
       </c>
     </row>
@@ -16230,7 +16383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{255CC822-9241-F641-95BA-C12DC3DE9827}">
   <dimension ref="A1:G502"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>

</xml_diff>